<commit_message>
added program to excel
</commit_message>
<xml_diff>
--- a/DS.xlsx
+++ b/DS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohitkunal\Desktop\F\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohitkunal\Desktop\DSAndAlgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB50C07-DAB6-4006-9267-E0D63072BBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9188A6E-6BE4-4BFC-843B-88D00E2B8445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
   </bookViews>
   <sheets>
     <sheet name="General problems" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="71">
   <si>
     <t>Problem Statement</t>
   </si>
@@ -246,10 +246,13 @@
     <t>This problem is similar to problem number 7, just k= j-i+1</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Suggestions</t>
+  </si>
+  <si>
+    <t>ReverseAStackUsingRecursion</t>
+  </si>
+  <si>
+    <t>Reverse a stack using recursion</t>
   </si>
 </sst>
 </file>
@@ -647,7 +650,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,15 +677,12 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -783,10 +783,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3383A26-CC4D-4749-8B3E-72875307696D}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -802,7 +802,7 @@
     <col min="9" max="9" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -813,25 +813,22 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44357</v>
       </c>
@@ -855,7 +852,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -881,15 +878,12 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -976,7 +970,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83486DE4-2450-4433-B065-ED9EE7E097B3}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -994,7 +988,7 @@
     <col min="8" max="8" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1005,19 +999,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44342</v>
       </c>
@@ -1028,7 +1019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44342</v>
       </c>
@@ -1039,7 +1030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44359</v>
       </c>
@@ -1060,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4177D779-440F-4A95-A73E-C867361DD890}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1077,7 +1068,7 @@
     <col min="8" max="8" width="22.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1088,23 +1079,20 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44359</v>
       </c>
@@ -1118,7 +1106,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44359</v>
       </c>
@@ -1130,6 +1118,20 @@
       </c>
       <c r="E3" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>44398</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1139,7 +1141,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707F8BA7-8667-494E-BF55-87BB02710AB7}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -1157,7 +1159,7 @@
     <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1168,23 +1170,20 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
     </row>
   </sheetData>
@@ -1196,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF7DBEA-E268-48C2-ABEB-72F1B2719E63}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1205,7 +1204,7 @@
     <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="31.36328125" customWidth="1"/>
+    <col min="5" max="5" width="35.54296875" customWidth="1"/>
     <col min="6" max="6" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
@@ -1223,19 +1222,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1363,7 +1359,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1379,7 +1375,7 @@
       <c r="F9" t="s">
         <v>53</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1406,10 +1402,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2082500-9E33-43A0-8947-BDCE4F2D37E7}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1423,7 +1419,7 @@
     <col min="8" max="8" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1434,19 +1430,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1454,7 +1447,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
DeleteMiddleElementOfAStack and KthSymbolInGrammar programs
</commit_message>
<xml_diff>
--- a/DS.xlsx
+++ b/DS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohitkunal\Desktop\DSAndAlgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9188A6E-6BE4-4BFC-843B-88D00E2B8445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7021199F-DEA4-4A94-BE2E-FE63A8058C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
   </bookViews>
   <sheets>
     <sheet name="General problems" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="75">
   <si>
     <t>Problem Statement</t>
   </si>
@@ -253,6 +253,18 @@
   </si>
   <si>
     <t>Reverse a stack using recursion</t>
+  </si>
+  <si>
+    <t>DeleteMiddleElementOfAStack</t>
+  </si>
+  <si>
+    <t>Delete middle element of a stack</t>
+  </si>
+  <si>
+    <t>KthSymbolInGrammar</t>
+  </si>
+  <si>
+    <t>Print Kth symbol in grammar</t>
   </si>
 </sst>
 </file>
@@ -647,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3527718D-AD0E-457D-A529-4FEC17308A97}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,6 +782,20 @@
       </c>
       <c r="E7" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>44399</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1051,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4177D779-440F-4A95-A73E-C867361DD890}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1132,6 +1158,20 @@
       </c>
       <c r="E4" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>44398</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Print subsets of a string
</commit_message>
<xml_diff>
--- a/DS.xlsx
+++ b/DS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohitkunal\Desktop\DSAndAlgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3A37CA-FDAD-4DC1-B8E6-0B48392589ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA97D30-DE1A-47DC-997D-A74135C9777D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
   </bookViews>
   <sheets>
     <sheet name="General problems" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="88">
   <si>
     <t>Problem Statement</t>
   </si>
@@ -274,6 +274,36 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=rf6uf3jNjbo</t>
+  </si>
+  <si>
+    <t>PrintSubsetsOfAString</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/print-subsequences-string/</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done - D</t>
+  </si>
+  <si>
+    <t>Done - R</t>
+  </si>
+  <si>
+    <t>Print all subsets and unique subsets of a string</t>
+  </si>
+  <si>
+    <t>Factorial</t>
+  </si>
+  <si>
+    <t>FibonacciSeries</t>
+  </si>
+  <si>
+    <t>Done - D/R</t>
+  </si>
+  <si>
+    <t>MinimumWindowSubstring</t>
   </si>
 </sst>
 </file>
@@ -337,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -345,7 +375,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -668,26 +697,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3527718D-AD0E-457D-A529-4FEC17308A97}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="66.1796875" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" customWidth="1"/>
-    <col min="7" max="7" width="22.6328125" customWidth="1"/>
-    <col min="8" max="8" width="58" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="52.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" customWidth="1"/>
+    <col min="5" max="5" width="24.6328125" customWidth="1"/>
+    <col min="6" max="6" width="24.54296875" customWidth="1"/>
+    <col min="7" max="7" width="24.81640625" customWidth="1"/>
+    <col min="8" max="8" width="32.54296875" customWidth="1"/>
+    <col min="9" max="9" width="58" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -695,19 +725,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <f>DATE(2021,5,26)</f>
         <v>44342</v>
@@ -716,6 +752,9 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
@@ -725,7 +764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <f>DATE(2021,5,26)</f>
         <v>44342</v>
@@ -734,6 +773,9 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
@@ -743,18 +785,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44342</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44348</v>
       </c>
@@ -762,10 +801,19 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44348</v>
       </c>
@@ -773,13 +821,22 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="E6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44357</v>
       </c>
@@ -787,13 +844,19 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44399</v>
       </c>
@@ -801,13 +864,19 @@
         <v>74</v>
       </c>
       <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
       <c r="E8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44399</v>
       </c>
@@ -815,13 +884,42 @@
         <v>75</v>
       </c>
       <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
       <c r="E9" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>44399</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -836,26 +934,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3383A26-CC4D-4749-8B3E-72875307696D}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" customWidth="1"/>
     <col min="2" max="2" width="37.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
-    <col min="6" max="6" width="33.54296875" customWidth="1"/>
-    <col min="7" max="7" width="17.08984375" customWidth="1"/>
-    <col min="8" max="8" width="20.08984375" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" customWidth="1"/>
+    <col min="5" max="5" width="26.6328125" customWidth="1"/>
+    <col min="6" max="6" width="30.7265625" customWidth="1"/>
+    <col min="7" max="7" width="33.54296875" customWidth="1"/>
+    <col min="8" max="8" width="27.1796875" customWidth="1"/>
+    <col min="9" max="9" width="20.08984375" customWidth="1"/>
+    <col min="10" max="10" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -863,25 +962,30 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44357</v>
       </c>
@@ -889,9 +993,12 @@
         <v>36</v>
       </c>
       <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -902,25 +1009,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B33FB3-33F7-4FA9-99A1-BFDBE6D2539D}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="53.08984375" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
     <col min="5" max="5" width="20.81640625" customWidth="1"/>
-    <col min="6" max="6" width="52.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52" customWidth="1"/>
+    <col min="6" max="6" width="33.6328125" customWidth="1"/>
+    <col min="7" max="7" width="52.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -928,19 +1036,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <f>DATE(2021,5,4)</f>
         <v>44320</v>
@@ -948,65 +1062,73 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44321</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44335</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44336</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1023,25 +1145,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83486DE4-2450-4433-B065-ED9EE7E097B3}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.08984375" customWidth="1"/>
-    <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" customWidth="1"/>
-    <col min="8" max="8" width="25.36328125" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="27.08984375" customWidth="1"/>
+    <col min="9" max="9" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1049,41 +1172,48 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44342</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44342</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44359</v>
       </c>
@@ -1091,6 +1221,9 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
@@ -1104,24 +1237,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4177D779-440F-4A95-A73E-C867361DD890}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="2" width="63.08984375" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="28.08984375" customWidth="1"/>
-    <col min="6" max="6" width="26.1796875" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" customWidth="1"/>
-    <col min="8" max="8" width="22.54296875" customWidth="1"/>
+    <col min="2" max="2" width="51.6328125" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="27.453125" customWidth="1"/>
+    <col min="6" max="6" width="28.08984375" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="30.36328125" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1129,23 +1263,28 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44359</v>
       </c>
@@ -1153,13 +1292,16 @@
         <v>38</v>
       </c>
       <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44359</v>
       </c>
@@ -1167,13 +1309,16 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44398</v>
       </c>
@@ -1181,13 +1326,16 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44398</v>
       </c>
@@ -1195,6 +1343,9 @@
         <v>72</v>
       </c>
       <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" t="s">
@@ -1208,25 +1359,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707F8BA7-8667-494E-BF55-87BB02710AB7}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" customWidth="1"/>
-    <col min="6" max="6" width="11.6328125" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="2" max="2" width="62.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="5" max="5" width="23.90625" customWidth="1"/>
+    <col min="6" max="6" width="23.1796875" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" customWidth="1"/>
+    <col min="8" max="8" width="24.6328125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1234,23 +1386,30 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
     </row>
   </sheetData>
@@ -1262,20 +1421,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF7DBEA-E268-48C2-ABEB-72F1B2719E63}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="35.54296875" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="5" max="5" width="31.26953125" customWidth="1"/>
+    <col min="6" max="6" width="29.90625" customWidth="1"/>
+    <col min="7" max="7" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.08984375" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
@@ -1286,18 +1446,21 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1309,6 +1472,9 @@
         <v>43</v>
       </c>
       <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
@@ -1326,6 +1492,9 @@
         <v>44</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
@@ -1343,6 +1512,9 @@
         <v>45</v>
       </c>
       <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
       <c r="E4" t="s">
@@ -1360,6 +1532,9 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" t="s">
@@ -1369,23 +1544,26 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="7" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1397,6 +1575,9 @@
         <v>47</v>
       </c>
       <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7" t="s">
@@ -1406,14 +1587,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>50</v>
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>44398</v>
       </c>
       <c r="B8" t="s">
         <v>66</v>
       </c>
       <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
         <v>58</v>
       </c>
       <c r="E8" t="s">
@@ -1426,7 +1610,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1434,6 +1618,9 @@
         <v>48</v>
       </c>
       <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
       <c r="E9" t="s">
@@ -1454,7 +1641,13 @@
         <v>49</v>
       </c>
       <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
         <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>87</v>
       </c>
       <c r="F10" t="s">
         <v>53</v>
@@ -1469,24 +1662,26 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2082500-9E33-43A0-8947-BDCE4F2D37E7}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="32.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
+    <col min="5" max="5" width="29.6328125" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" customWidth="1"/>
+    <col min="7" max="7" width="32.90625" customWidth="1"/>
+    <col min="8" max="8" width="25.54296875" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1494,19 +1689,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1514,7 +1715,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
permutation problems with pick and don't pick way
</commit_message>
<xml_diff>
--- a/DS.xlsx
+++ b/DS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohitkunal\Desktop\DSAndAlgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA97D30-DE1A-47DC-997D-A74135C9777D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED79A568-03E1-4FBC-AC13-321E471B122C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
   </bookViews>
   <sheets>
     <sheet name="General problems" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="93">
   <si>
     <t>Problem Statement</t>
   </si>
@@ -304,6 +304,21 @@
   </si>
   <si>
     <t>MinimumWindowSubstring</t>
+  </si>
+  <si>
+    <t>Permutation of adding spaces in between of a string</t>
+  </si>
+  <si>
+    <t>PermutationWithSpaces</t>
+  </si>
+  <si>
+    <t>Permutation of changing case in a string</t>
+  </si>
+  <si>
+    <t>LetterCasePermutation</t>
+  </si>
+  <si>
+    <t>Permutation of string containing both alphabets and numbers. Case of alphabets will be toggled and numbers will be copied as it is.</t>
   </si>
 </sst>
 </file>
@@ -697,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3527718D-AD0E-457D-A529-4FEC17308A97}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,6 +935,66 @@
       </c>
       <c r="G10" s="3" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>44399</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>44399</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>44399</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1421,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF7DBEA-E268-48C2-ABEB-72F1B2719E63}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1664,7 +1739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2082500-9E33-43A0-8947-BDCE4F2D37E7}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Print binary number and Josephus problem
</commit_message>
<xml_diff>
--- a/DS.xlsx
+++ b/DS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohitkunal\Desktop\DSAndAlgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9898506-713E-476E-BB1E-B01A33865E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CC8E69-4E55-4E8D-B32D-A472F1893636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="99">
   <si>
     <t>Problem Statement</t>
   </si>
@@ -325,6 +325,18 @@
   </si>
   <si>
     <t>GenerateAllBalancedParenthesis</t>
+  </si>
+  <si>
+    <t>Print N digit binary number where 1s&gt;=0s in all its prefixes</t>
+  </si>
+  <si>
+    <t>PrintNDigitBinaryNumberWhereOnesGreaterThanEqualsToZeros</t>
+  </si>
+  <si>
+    <t>Josephus problem (Circle of death)</t>
+  </si>
+  <si>
+    <t>JosephusProblem</t>
   </si>
 </sst>
 </file>
@@ -718,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3527718D-AD0E-457D-A529-4FEC17308A97}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1020,6 +1032,46 @@
         <v>94</v>
       </c>
       <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>44400</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>44400</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nearest greater/smaller to right/left
</commit_message>
<xml_diff>
--- a/DS.xlsx
+++ b/DS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohitkunal\Desktop\DSAndAlgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CC8E69-4E55-4E8D-B32D-A472F1893636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754914A7-4D80-40BF-A059-23F831F5B91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{AC027467-1FEB-42DB-9976-384BB29FD753}"/>
   </bookViews>
   <sheets>
     <sheet name="General problems" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="103">
   <si>
     <t>Problem Statement</t>
   </si>
@@ -337,6 +337,20 @@
   </si>
   <si>
     <t>JosephusProblem</t>
+  </si>
+  <si>
+    <t>Nearest greater to right/left</t>
+  </si>
+  <si>
+    <t>NearestGreaterToRight
+NearestGreaterToLeft</t>
+  </si>
+  <si>
+    <t>Nearest smaller to right/left</t>
+  </si>
+  <si>
+    <t>NearestSmallerToRight
+NearestSmallerToLeft</t>
   </si>
 </sst>
 </file>
@@ -732,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3527718D-AD0E-457D-A529-4FEC17308A97}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1390,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4177D779-440F-4A95-A73E-C867361DD890}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1504,6 +1518,43 @@
       <c r="E5" t="s">
         <v>71</v>
       </c>
+    </row>
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>44406</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>44407</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>